<commit_message>
Updated the javadoc documentation comments
</commit_message>
<xml_diff>
--- a/TextTransformer.xlsx
+++ b/TextTransformer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frostyl\Repozytoria\Text-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDD2F1F-EA63-44D2-A8F7-B1900CACC3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3ADA23-9FDF-4553-80EC-A84A6F3C78BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opis" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>Element rejestru produktu</t>
   </si>
@@ -424,6 +424,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>108856</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>745952</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>46885</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obraz 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4380BBC1-D5B0-00ED-C033-512C3261146B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8153400" y="533399"/>
+          <a:ext cx="8638095" cy="5914286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -774,29 +823,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="95.5" customWidth="1"/>
+    <col min="3" max="3" width="25.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1001,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>